<commit_message>
Q2 is proper good
</commit_message>
<xml_diff>
--- a/Answers/E2ProteinsMST.xlsx
+++ b/Answers/E2ProteinsMST.xlsx
@@ -436,609 +436,609 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>('ANG_1',)</t>
+          <t>ANG_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>('BDNF_1',)</t>
+          <t>BDNF_1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>('BLC_1',)</t>
+          <t>BLC_1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>('BMP-4_1',)</t>
+          <t>BMP-4_1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>('BMP-6_1',)</t>
+          <t>BMP-6_1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>('CK b8-1_1',)</t>
+          <t>CK b8-1_1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>('CNTF_1',)</t>
+          <t>CNTF_1</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>('EGF_1',)</t>
+          <t>EGF_1</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>('Eotaxin_1',)</t>
+          <t>Eotaxin_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>('Eotaxin-2_1',)</t>
+          <t>Eotaxin-2_1</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>('Eotaxin-3_1',)</t>
+          <t>Eotaxin-3_1</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>('FGF-6_1',)</t>
+          <t>FGF-6_1</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>('FGF-7_1',)</t>
+          <t>FGF-7_1</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>('Fit-3 Ligand_1',)</t>
+          <t>Fit-3 Ligand_1</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>('Fractalkine_1',)</t>
+          <t>Fractalkine_1</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>('GCP-2_1',)</t>
+          <t>GCP-2_1</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>('GDNF_1',)</t>
+          <t>GDNF_1</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>('GM-CSF_1',)</t>
+          <t>GM-CSF_1</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>('I-309_1',)</t>
+          <t>I-309_1</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>('IFN-g_1',)</t>
+          <t>IFN-g_1</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>('IGF-1_1',)</t>
+          <t>IGF-1_1</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-1_1',)</t>
+          <t>IGFBP-1_1</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-2_1',)</t>
+          <t>IGFBP-2_1</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-4_1',)</t>
+          <t>IGFBP-4_1</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>('IL-10_1',)</t>
+          <t>IL-10_1</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>('IL-13_1',)</t>
+          <t>IL-13_1</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>('IL-15_1',)</t>
+          <t>IL-15_1</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>('IL-16_1',)</t>
+          <t>IL-16_1</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>('IL-1a_1',)</t>
+          <t>IL-1a_1</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>('IL-1b_1',)</t>
+          <t>IL-1b_1</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>('IL-1ra_1',)</t>
+          <t>IL-1ra_1</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>('IL-2_1',)</t>
+          <t>IL-2_1</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>('IL-3_1',)</t>
+          <t>IL-3_1</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>('IL-4_1',)</t>
+          <t>IL-4_1</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>('IL-5_1',)</t>
+          <t>IL-5_1</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>('IL-6_1',)</t>
+          <t>IL-6_1</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>('IL-7_1',)</t>
+          <t>IL-7_1</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>('LEPTIN(OB)_1',)</t>
+          <t>LEPTIN(OB)_1</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>('LIGHT_1',)</t>
+          <t>LIGHT_1</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>('MCP-1_1',)</t>
+          <t>MCP-1_1</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>('MCP-2_1',)</t>
+          <t>MCP-2_1</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>('MCP-3_1',)</t>
+          <t>MCP-3_1</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>('MCP-4_1',)</t>
+          <t>MCP-4_1</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>('M-CSF_1',)</t>
+          <t>M-CSF_1</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>('MDC_1',)</t>
+          <t>MDC_1</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>('MIG_1',)</t>
+          <t>MIG_1</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>('MIP-1d_1',)</t>
+          <t>MIP-1d_1</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>('MIP-3a_1',)</t>
+          <t>MIP-3a_1</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>('NAP-2_1',)</t>
+          <t>NAP-2_1</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>('NT-3_1',)</t>
+          <t>NT-3_1</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>('PARC_1',)</t>
+          <t>PARC_1</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>('PDGF-BB_1',)</t>
+          <t>PDGF-BB_1</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>('RANTES_1',)</t>
+          <t>RANTES_1</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>('SCF_1',)</t>
+          <t>SCF_1</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>('SDF-1_1',)</t>
+          <t>SDF-1_1</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>('TARC_1',)</t>
+          <t>TARC_1</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>('TGF-b_1',)</t>
+          <t>TGF-b_1</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>('TGF-b3_1',)</t>
+          <t>TGF-b3_1</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>('TNF-a_1',)</t>
+          <t>TNF-a_1</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>('TNF-b_1',)</t>
+          <t>TNF-b_1</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>('Acrp30_1',)</t>
+          <t>Acrp30_1</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>('AgRP(ART)_1',)</t>
+          <t>AgRP(ART)_1</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>('ANG-2_1',)</t>
+          <t>ANG-2_1</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>('AR_1',)</t>
+          <t>AR_1</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>('AXL_1',)</t>
+          <t>AXL_1</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>('bFGF',)</t>
+          <t>bFGF</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>('b-NGF_1',)</t>
+          <t>b-NGF_1</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>('BTC_1',)</t>
+          <t>BTC_1</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>('CCL-28_1',)</t>
+          <t>CCL-28_1</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>('CTACK_1',)</t>
+          <t>CTACK_1</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>('DTK_1',)</t>
+          <t>DTK_1</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>('EGF-R_1',)</t>
+          <t>EGF-R_1</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>('ENA-78_1',)</t>
+          <t>ENA-78_1</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>('FAS_1',)</t>
+          <t>FAS_1</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>('FGF-4_1',)</t>
+          <t>FGF-4_1</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>('FGF-9_1',)</t>
+          <t>FGF-9_1</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
-          <t>('GCSF_1',)</t>
+          <t>GCSF_1</t>
         </is>
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>('GITR_1',)</t>
+          <t>GITR_1</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>('GITR-Light_1',)</t>
+          <t>GITR-Light_1</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>('GRO_1',)</t>
+          <t>GRO_1</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>('GRO-a_1',)</t>
+          <t>GRO-a_1</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>('HCC-4_1',)</t>
+          <t>HCC-4_1</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>('HGF_1',)</t>
+          <t>HGF_1</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>('ICAM-1_1',)</t>
+          <t>ICAM-1_1</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
         <is>
-          <t>('ICAM-3_1',)</t>
+          <t>ICAM-3_1</t>
         </is>
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>('IGF-1 SR',)</t>
+          <t>IGF-1 SR</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP3_1',)</t>
+          <t>IGFBP3_1</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-6_1',)</t>
+          <t>IGFBP-6_1</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>('IL-1 RI_1',)</t>
+          <t>IL-1 RI_1</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>('IL-11_1',)</t>
+          <t>IL-11_1</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
         <is>
-          <t>('IL-12 p40_1',)</t>
+          <t>IL-12 p40_1</t>
         </is>
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>('IL-12 p70_1',)</t>
+          <t>IL-12 p70_1</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>('IL-17_1',)</t>
+          <t>IL-17_1</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>('IL-1R4 /ST2_1',)</t>
+          <t>IL-1R4 /ST2_1</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>('IL-2 Ra_1',)</t>
+          <t>IL-2 Ra_1</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>('IL-6 R_1',)</t>
+          <t>IL-6 R_1</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
         <is>
-          <t>('IL-8_1',)</t>
+          <t>IL-8_1</t>
         </is>
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>('I-TAC_1',)</t>
+          <t>I-TAC_1</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
         <is>
-          <t>('Lymphotactin_1',)</t>
+          <t>Lymphotactin_1</t>
         </is>
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>('MIF_1',)</t>
+          <t>MIF_1</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>('MIP-1a_1',)</t>
+          <t>MIP-1a_1</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>('MIP-1b_1',)</t>
+          <t>MIP-1b_1</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>('MIP-3b_1',)</t>
+          <t>MIP-3b_1</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>('MSP-a_1',)</t>
+          <t>MSP-a_1</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>('NT-4_1',)</t>
+          <t>NT-4_1</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>('OSM_1',)</t>
+          <t>OSM_1</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>('OST_1',)</t>
+          <t>OST_1</t>
         </is>
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>('PIGF_1',)</t>
+          <t>PIGF_1</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
-          <t>('spg130_1',)</t>
+          <t>spg130_1</t>
         </is>
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>('sTNF RI_1',)</t>
+          <t>sTNF RI_1</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
         <is>
-          <t>('sTNF RII_1',)</t>
+          <t>sTNF RII_1</t>
         </is>
       </c>
       <c r="DI1" s="1" t="inlineStr">
         <is>
-          <t>('TECK_1',)</t>
+          <t>TECK_1</t>
         </is>
       </c>
       <c r="DJ1" s="1" t="inlineStr">
         <is>
-          <t>('TIMP-1_1',)</t>
+          <t>TIMP-1_1</t>
         </is>
       </c>
       <c r="DK1" s="1" t="inlineStr">
         <is>
-          <t>('TIMP-2_1',)</t>
+          <t>TIMP-2_1</t>
         </is>
       </c>
       <c r="DL1" s="1" t="inlineStr">
         <is>
-          <t>('TPO_1',)</t>
+          <t>TPO_1</t>
         </is>
       </c>
       <c r="DM1" s="1" t="inlineStr">
         <is>
-          <t>('TRAIL R3_1',)</t>
+          <t>TRAIL R3_1</t>
         </is>
       </c>
       <c r="DN1" s="1" t="inlineStr">
         <is>
-          <t>('TRAIL R4_1',)</t>
+          <t>TRAIL R4_1</t>
         </is>
       </c>
       <c r="DO1" s="1" t="inlineStr">
         <is>
-          <t>('uPAR_1',)</t>
+          <t>uPAR_1</t>
         </is>
       </c>
       <c r="DP1" s="1" t="inlineStr">
         <is>
-          <t>('VEGF-B_1',)</t>
+          <t>VEGF-B_1</t>
         </is>
       </c>
       <c r="DQ1" s="1" t="inlineStr">
         <is>
-          <t>('VEGF-D_1',)</t>
+          <t>VEGF-D_1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>('ANG_1',)</t>
+          <t>ANG_1</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1405,7 +1405,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>('BDNF_1',)</t>
+          <t>BDNF_1</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1772,7 +1772,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>('BLC_1',)</t>
+          <t>BLC_1</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2139,7 +2139,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>('BMP-4_1',)</t>
+          <t>BMP-4_1</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2506,7 +2506,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>('BMP-6_1',)</t>
+          <t>BMP-6_1</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2873,7 +2873,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>('CK b8-1_1',)</t>
+          <t>CK b8-1_1</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3240,7 +3240,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>('CNTF_1',)</t>
+          <t>CNTF_1</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3607,7 +3607,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>('EGF_1',)</t>
+          <t>EGF_1</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -3974,7 +3974,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>('Eotaxin_1',)</t>
+          <t>Eotaxin_1</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4341,7 +4341,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>('Eotaxin-2_1',)</t>
+          <t>Eotaxin-2_1</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -4708,7 +4708,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>('Eotaxin-3_1',)</t>
+          <t>Eotaxin-3_1</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -5075,7 +5075,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>('FGF-6_1',)</t>
+          <t>FGF-6_1</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -5442,7 +5442,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>('FGF-7_1',)</t>
+          <t>FGF-7_1</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -5809,7 +5809,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>('Fit-3 Ligand_1',)</t>
+          <t>Fit-3 Ligand_1</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -6176,7 +6176,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>('Fractalkine_1',)</t>
+          <t>Fractalkine_1</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -6543,7 +6543,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>('GCP-2_1',)</t>
+          <t>GCP-2_1</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -6910,7 +6910,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>('GDNF_1',)</t>
+          <t>GDNF_1</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -7277,7 +7277,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>('GM-CSF_1',)</t>
+          <t>GM-CSF_1</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -7644,7 +7644,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>('I-309_1',)</t>
+          <t>I-309_1</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -8011,7 +8011,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>('IFN-g_1',)</t>
+          <t>IFN-g_1</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -8378,7 +8378,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>('IGF-1_1',)</t>
+          <t>IGF-1_1</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -8745,7 +8745,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-1_1',)</t>
+          <t>IGFBP-1_1</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -9112,7 +9112,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-2_1',)</t>
+          <t>IGFBP-2_1</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -9479,7 +9479,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-4_1',)</t>
+          <t>IGFBP-4_1</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -9846,7 +9846,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>('IL-10_1',)</t>
+          <t>IL-10_1</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -10213,7 +10213,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>('IL-13_1',)</t>
+          <t>IL-13_1</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -10580,7 +10580,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>('IL-15_1',)</t>
+          <t>IL-15_1</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -10947,7 +10947,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>('IL-16_1',)</t>
+          <t>IL-16_1</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -11314,7 +11314,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>('IL-1a_1',)</t>
+          <t>IL-1a_1</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -11681,7 +11681,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>('IL-1b_1',)</t>
+          <t>IL-1b_1</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -12048,7 +12048,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>('IL-1ra_1',)</t>
+          <t>IL-1ra_1</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -12415,7 +12415,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>('IL-2_1',)</t>
+          <t>IL-2_1</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -12782,7 +12782,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>('IL-3_1',)</t>
+          <t>IL-3_1</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -13149,7 +13149,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>('IL-4_1',)</t>
+          <t>IL-4_1</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -13516,7 +13516,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>('IL-5_1',)</t>
+          <t>IL-5_1</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -13883,7 +13883,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>('IL-6_1',)</t>
+          <t>IL-6_1</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -14250,7 +14250,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>('IL-7_1',)</t>
+          <t>IL-7_1</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -14617,7 +14617,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>('LEPTIN(OB)_1',)</t>
+          <t>LEPTIN(OB)_1</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -14984,7 +14984,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>('LIGHT_1',)</t>
+          <t>LIGHT_1</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -15351,7 +15351,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>('MCP-1_1',)</t>
+          <t>MCP-1_1</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -15718,7 +15718,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>('MCP-2_1',)</t>
+          <t>MCP-2_1</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -16085,7 +16085,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>('MCP-3_1',)</t>
+          <t>MCP-3_1</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -16452,7 +16452,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>('MCP-4_1',)</t>
+          <t>MCP-4_1</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -16819,7 +16819,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>('M-CSF_1',)</t>
+          <t>M-CSF_1</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -17186,7 +17186,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>('MDC_1',)</t>
+          <t>MDC_1</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -17553,7 +17553,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>('MIG_1',)</t>
+          <t>MIG_1</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -17920,7 +17920,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>('MIP-1d_1',)</t>
+          <t>MIP-1d_1</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -18287,7 +18287,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>('MIP-3a_1',)</t>
+          <t>MIP-3a_1</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -18654,7 +18654,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>('NAP-2_1',)</t>
+          <t>NAP-2_1</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -19021,7 +19021,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>('NT-3_1',)</t>
+          <t>NT-3_1</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -19388,7 +19388,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>('PARC_1',)</t>
+          <t>PARC_1</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -19755,7 +19755,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>('PDGF-BB_1',)</t>
+          <t>PDGF-BB_1</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -20122,7 +20122,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>('RANTES_1',)</t>
+          <t>RANTES_1</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -20489,7 +20489,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>('SCF_1',)</t>
+          <t>SCF_1</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -20856,7 +20856,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>('SDF-1_1',)</t>
+          <t>SDF-1_1</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -21223,7 +21223,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>('TARC_1',)</t>
+          <t>TARC_1</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -21590,7 +21590,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>('TGF-b_1',)</t>
+          <t>TGF-b_1</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -21957,7 +21957,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>('TGF-b3_1',)</t>
+          <t>TGF-b3_1</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -22324,7 +22324,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>('TNF-a_1',)</t>
+          <t>TNF-a_1</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -22691,7 +22691,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>('TNF-b_1',)</t>
+          <t>TNF-b_1</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -23058,7 +23058,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>('Acrp30_1',)</t>
+          <t>Acrp30_1</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -23425,7 +23425,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>('AgRP(ART)_1',)</t>
+          <t>AgRP(ART)_1</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -23792,7 +23792,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>('ANG-2_1',)</t>
+          <t>ANG-2_1</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -24159,7 +24159,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>('AR_1',)</t>
+          <t>AR_1</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -24526,7 +24526,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>('AXL_1',)</t>
+          <t>AXL_1</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -24893,7 +24893,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>('bFGF',)</t>
+          <t>bFGF</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -25260,7 +25260,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>('b-NGF_1',)</t>
+          <t>b-NGF_1</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -25627,7 +25627,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>('BTC_1',)</t>
+          <t>BTC_1</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -25994,7 +25994,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>('CCL-28_1',)</t>
+          <t>CCL-28_1</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -26361,7 +26361,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>('CTACK_1',)</t>
+          <t>CTACK_1</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -26728,7 +26728,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>('DTK_1',)</t>
+          <t>DTK_1</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -27095,7 +27095,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>('EGF-R_1',)</t>
+          <t>EGF-R_1</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -27462,7 +27462,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>('ENA-78_1',)</t>
+          <t>ENA-78_1</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -27829,7 +27829,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>('FAS_1',)</t>
+          <t>FAS_1</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -28196,7 +28196,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>('FGF-4_1',)</t>
+          <t>FGF-4_1</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -28563,7 +28563,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>('FGF-9_1',)</t>
+          <t>FGF-9_1</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -28930,7 +28930,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>('GCSF_1',)</t>
+          <t>GCSF_1</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -29297,7 +29297,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>('GITR_1',)</t>
+          <t>GITR_1</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -29664,7 +29664,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>('GITR-Light_1',)</t>
+          <t>GITR-Light_1</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -30031,7 +30031,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>('GRO_1',)</t>
+          <t>GRO_1</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -30398,7 +30398,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>('GRO-a_1',)</t>
+          <t>GRO-a_1</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -30765,7 +30765,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>('HCC-4_1',)</t>
+          <t>HCC-4_1</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -31132,7 +31132,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>('HGF_1',)</t>
+          <t>HGF_1</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -31499,7 +31499,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>('ICAM-1_1',)</t>
+          <t>ICAM-1_1</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -31866,7 +31866,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>('ICAM-3_1',)</t>
+          <t>ICAM-3_1</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -32233,7 +32233,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>('IGF-1 SR',)</t>
+          <t>IGF-1 SR</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -32600,7 +32600,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP3_1',)</t>
+          <t>IGFBP3_1</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -32967,7 +32967,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>('IGFBP-6_1',)</t>
+          <t>IGFBP-6_1</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -33334,7 +33334,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>('IL-1 RI_1',)</t>
+          <t>IL-1 RI_1</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -33701,7 +33701,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>('IL-11_1',)</t>
+          <t>IL-11_1</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -34068,7 +34068,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>('IL-12 p40_1',)</t>
+          <t>IL-12 p40_1</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -34435,7 +34435,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>('IL-12 p70_1',)</t>
+          <t>IL-12 p70_1</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -34802,7 +34802,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>('IL-17_1',)</t>
+          <t>IL-17_1</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -35169,7 +35169,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>('IL-1R4 /ST2_1',)</t>
+          <t>IL-1R4 /ST2_1</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -35536,7 +35536,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>('IL-2 Ra_1',)</t>
+          <t>IL-2 Ra_1</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -35903,7 +35903,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>('IL-6 R_1',)</t>
+          <t>IL-6 R_1</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -36270,7 +36270,7 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>('IL-8_1',)</t>
+          <t>IL-8_1</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -36637,7 +36637,7 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>('I-TAC_1',)</t>
+          <t>I-TAC_1</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -37004,7 +37004,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>('Lymphotactin_1',)</t>
+          <t>Lymphotactin_1</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -37371,7 +37371,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>('MIF_1',)</t>
+          <t>MIF_1</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -37738,7 +37738,7 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>('MIP-1a_1',)</t>
+          <t>MIP-1a_1</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -38105,7 +38105,7 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>('MIP-1b_1',)</t>
+          <t>MIP-1b_1</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -38472,7 +38472,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>('MIP-3b_1',)</t>
+          <t>MIP-3b_1</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -38839,7 +38839,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>('MSP-a_1',)</t>
+          <t>MSP-a_1</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -39206,7 +39206,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>('NT-4_1',)</t>
+          <t>NT-4_1</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -39573,7 +39573,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>('OSM_1',)</t>
+          <t>OSM_1</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -39940,7 +39940,7 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>('OST_1',)</t>
+          <t>OST_1</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -40307,7 +40307,7 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>('PIGF_1',)</t>
+          <t>PIGF_1</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -40674,7 +40674,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>('spg130_1',)</t>
+          <t>spg130_1</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -41041,7 +41041,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>('sTNF RI_1',)</t>
+          <t>sTNF RI_1</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -41408,7 +41408,7 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>('sTNF RII_1',)</t>
+          <t>sTNF RII_1</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -41775,7 +41775,7 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>('TECK_1',)</t>
+          <t>TECK_1</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -42142,7 +42142,7 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>('TIMP-1_1',)</t>
+          <t>TIMP-1_1</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -42509,7 +42509,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>('TIMP-2_1',)</t>
+          <t>TIMP-2_1</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -42876,7 +42876,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>('TPO_1',)</t>
+          <t>TPO_1</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -43243,7 +43243,7 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>('TRAIL R3_1',)</t>
+          <t>TRAIL R3_1</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -43610,7 +43610,7 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>('TRAIL R4_1',)</t>
+          <t>TRAIL R4_1</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -43977,7 +43977,7 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>('uPAR_1',)</t>
+          <t>uPAR_1</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -44344,7 +44344,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>('VEGF-B_1',)</t>
+          <t>VEGF-B_1</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -44711,7 +44711,7 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>('VEGF-D_1',)</t>
+          <t>VEGF-D_1</t>
         </is>
       </c>
       <c r="B121" t="n">

</xml_diff>